<commit_message>
1. Se crean alguno casos de prueba 2. Se genera la columna de duración estimada en el project (pero no funciona)
</commit_message>
<xml_diff>
--- a/se/Trabajo Profesional/Disciplinas/Aseguramiento de la Calidad/AC - Template Casos de Prueba.xlsx
+++ b/se/Trabajo Profesional/Disciplinas/Aseguramiento de la Calidad/AC - Template Casos de Prueba.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="18990" windowHeight="8280"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>VARIACIONES</t>
   </si>
@@ -159,6 +159,105 @@
   </si>
   <si>
     <t>Datos</t>
+  </si>
+  <si>
+    <t>1. Seleccionar 'register'
+2. Presionar el botón 'Send'</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Registrando usuario</t>
+  </si>
+  <si>
+    <t>1. Seleccionar 'register'
+2. Seleccionar tipo de licencia 'Select License'
+3. Completar mail
+4. Presionar el botón 'Send'</t>
+  </si>
+  <si>
+    <t>Critico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar:
+1. Que se informa por pantalla que se registro el alta
+2. Que se envio el mail a la casilla ingresada
+3. Que el usuario existe en la BD </t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema informa por pantalla  que faltan datos obligatorios</t>
+  </si>
+  <si>
+    <t>1. Seleccionar 'register'
+2. Seleccionar tipo de licencia 'Select License'
+3. Presionar el botón 'Send'</t>
+  </si>
+  <si>
+    <t>1. Seleccionar 'register'
+2. Completar mail
+3. Presionar el botón 'Send'</t>
+  </si>
+  <si>
+    <t>Ingresando al sistema</t>
+  </si>
+  <si>
+    <t>1. Ingresar usuario
+2. Ingresar password
+3. Presionar el botón 'Send'</t>
+  </si>
+  <si>
+    <t>Verificar que el usuario se logueo al sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresando al sistema </t>
+  </si>
+  <si>
+    <t>Usuario existente</t>
+  </si>
+  <si>
+    <t>Usuario inexistente</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema informa por pantalla que el usuario no existe</t>
+  </si>
+  <si>
+    <t>Usuario existente - password incorrecto</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema informa por pantalla que los datos ingresados son incorrecto</t>
+  </si>
+  <si>
+    <t>Validando licencia faltante</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validando email faltante</t>
+  </si>
+  <si>
+    <t>Validando datos faltante</t>
+  </si>
+  <si>
+    <t>Solicitando contraseña</t>
+  </si>
+  <si>
+    <t>1. Seleccionar 'lost password?'
+2. Completar mail
+3. Presionar el botón 'Send'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar:
+1. Que se informa por pantalla que la accion se realizo exitosamente
+2. Que se envio el mail a la casilla ingresada
+3. Que al usuario se le modifico la password en la BD </t>
   </si>
 </sst>
 </file>
@@ -429,9 +528,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -439,19 +544,229 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -797,21 +1112,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1048576"/>
+  <dimension ref="A1:P1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1"/>
     <col min="6" max="6" width="46" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" style="15" customWidth="1"/>
@@ -826,25 +1141,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="31" t="s">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="31"/>
+      <c r="I1" s="29"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="30"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -869,8 +1184,8 @@
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="16"/>
       <c r="K2" s="6" t="s">
         <v>12</v>
@@ -889,52 +1204,86 @@
       </c>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="17"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="1"/>
       <c r="K3" s="26"/>
       <c r="L3" s="14"/>
       <c r="M3" s="19"/>
       <c r="N3" s="18"/>
       <c r="O3" s="11"/>
-      <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="1"/>
       <c r="K4" s="26"/>
       <c r="L4" s="14"/>
       <c r="M4" s="19"/>
       <c r="N4" s="18"/>
       <c r="O4" s="11"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="17"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="1"/>
       <c r="K5" s="26"/>
       <c r="L5" s="14"/>
@@ -943,16 +1292,28 @@
       <c r="O5" s="11"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="1"/>
       <c r="K6" s="26"/>
       <c r="L6" s="14"/>
@@ -961,14 +1322,26 @@
       <c r="O6" s="11"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="17"/>
       <c r="J7" s="1"/>
@@ -979,34 +1352,58 @@
       <c r="O7" s="11"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="17"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="26"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="14"/>
       <c r="M8" s="19"/>
       <c r="N8" s="18"/>
       <c r="O8" s="11"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="17"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="1"/>
       <c r="K9" s="7"/>
       <c r="L9" s="14"/>
@@ -1015,16 +1412,26 @@
       <c r="O9" s="11"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="1"/>
       <c r="K10" s="7"/>
       <c r="L10" s="14"/>
@@ -1039,10 +1446,10 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="17"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="1"/>
       <c r="K11" s="7"/>
       <c r="L11" s="14"/>
@@ -1057,10 +1464,10 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="1"/>
       <c r="K12" s="7"/>
       <c r="L12" s="14"/>
@@ -1075,7 +1482,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3"/>
       <c r="I13" s="17"/>
@@ -1093,7 +1500,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="17"/>
@@ -1111,7 +1518,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="17"/>
@@ -1120,7 +1527,7 @@
       <c r="L15" s="14"/>
       <c r="M15" s="19"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="11"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1129,7 +1536,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3"/>
       <c r="I16" s="17"/>
@@ -1147,7 +1554,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="2"/>
       <c r="H17" s="3"/>
       <c r="I17" s="17"/>
@@ -1156,8 +1563,8 @@
       <c r="L17" s="14"/>
       <c r="M17" s="19"/>
       <c r="N17" s="18"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="1"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
@@ -1175,7 +1582,7 @@
       <c r="M18" s="19"/>
       <c r="N18" s="18"/>
       <c r="O18" s="11"/>
-      <c r="P18" s="8"/>
+      <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
@@ -1198,7 +1605,7 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1252,7 +1659,7 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="9"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1262,9 +1669,9 @@
       <c r="J23" s="1"/>
       <c r="K23" s="7"/>
       <c r="L23" s="14"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="11"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="10"/>
       <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -1295,29 +1702,22 @@
       <c r="G25" s="2"/>
       <c r="H25" s="3"/>
       <c r="I25" s="17"/>
-      <c r="J25" s="1"/>
       <c r="K25" s="7"/>
       <c r="L25" s="14"/>
       <c r="M25" s="20"/>
       <c r="N25" s="17"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="1"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="17"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="10"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
@@ -1364,15 +1764,7 @@
       <c r="I30" s="23"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="23"/>
+      <c r="A31" s="25"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
@@ -1381,22 +1773,19 @@
       <c r="A33" s="25"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="24"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-    </row>
-    <row r="1048576" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1048576" s="2"/>
+    <row r="1048575" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1048575" s="2"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="J3:J4 K3:P17 J18:P19 K20:P25 H3:I31 K26:O26" name="datos variaciones"/>
+    <protectedRange sqref="J17:P18 K19:P24 H3:P4 K25:O25 K5:P16 H5:I30" name="datos variaciones"/>
     <protectedRange sqref="H2:J2" name="encabezado variaciones"/>
-    <protectedRange sqref="F1048576 A3:G31" name="Datos basicos TC"/>
+    <protectedRange sqref="F1048575:F1048576 A3:G30" name="Datos basicos TC"/>
   </protectedRanges>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
@@ -1404,24 +1793,24 @@
     <mergeCell ref="K1:O1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="3" priority="178" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="G2:G3 G7:G30">
+    <cfRule type="cellIs" dxfId="17" priority="189" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="179" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="190" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N26">
-    <cfRule type="cellIs" dxfId="1" priority="176" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N5:N25 N2:N3">
+    <cfRule type="cellIs" dxfId="15" priority="187" stopIfTrue="1" operator="equal">
       <formula>"TEST OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="177" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="188" stopIfTrue="1" operator="equal">
       <formula>"TEST FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22">
-    <cfRule type="iconSet" priority="170">
+  <conditionalFormatting sqref="G21">
+    <cfRule type="iconSet" priority="181">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1429,8 +1818,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23">
-    <cfRule type="iconSet" priority="165">
+  <conditionalFormatting sqref="G22">
+    <cfRule type="iconSet" priority="176">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1438,8 +1827,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24">
-    <cfRule type="iconSet" priority="160">
+  <conditionalFormatting sqref="G23">
+    <cfRule type="iconSet" priority="171">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1447,8 +1836,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G25">
-    <cfRule type="iconSet" priority="155">
+  <conditionalFormatting sqref="G24">
+    <cfRule type="iconSet" priority="166">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1456,8 +1845,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
-    <cfRule type="iconSet" priority="150">
+  <conditionalFormatting sqref="G25">
+    <cfRule type="iconSet" priority="161">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1465,8 +1854,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:G26">
-    <cfRule type="iconSet" priority="76">
+  <conditionalFormatting sqref="G23:G25">
+    <cfRule type="iconSet" priority="87">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1474,8 +1863,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
-    <cfRule type="iconSet" priority="55">
+  <conditionalFormatting sqref="G26">
+    <cfRule type="iconSet" priority="66">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1483,8 +1872,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="iconSet" priority="49">
+  <conditionalFormatting sqref="G27">
+    <cfRule type="iconSet" priority="60">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1492,8 +1881,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G29">
-    <cfRule type="iconSet" priority="43">
+  <conditionalFormatting sqref="G28">
+    <cfRule type="iconSet" priority="54">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1501,8 +1890,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
-    <cfRule type="iconSet" priority="37">
+  <conditionalFormatting sqref="G29">
+    <cfRule type="iconSet" priority="48">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1510,8 +1899,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="iconSet" priority="31">
+  <conditionalFormatting sqref="G30">
+    <cfRule type="iconSet" priority="42">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1519,8 +1908,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G21">
-    <cfRule type="iconSet" priority="201">
+  <conditionalFormatting sqref="G3 G7:G20">
+    <cfRule type="iconSet" priority="212">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1528,17 +1917,76 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="cellIs" dxfId="13" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"True"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"False"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4">
+    <cfRule type="cellIs" dxfId="11" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"TEST OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"TEST FAIL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"True"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"False"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="iconSet" priority="6">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"True"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"False"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M25">
       <formula1>"Sin ejecutar,Ejecutado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N25">
       <formula1>"TEST OK, TEST FAIL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E30">
       <formula1>"Critico,Alto,Bajo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G30">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>